<commit_message>
import excel sheet update
</commit_message>
<xml_diff>
--- a/data/complete_questions.xlsx
+++ b/data/complete_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation-Project\graduation-project--master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\graduation-project--master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFEBD81-0E8D-40EB-88B6-9226F11330C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A4A502-1F9F-4D5C-A968-A3EEED07B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D149FCC7-2006-47E0-B465-8BD4EC32FBC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D149FCC7-2006-47E0-B465-8BD4EC32FBC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>question</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>course_id</t>
   </si>
   <si>
     <t xml:space="preserve"> Hyper Text Markup Language</t>
@@ -434,20 +431,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B492C82-F2A3-4888-8E5C-8D9CFB19A6C1}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="F1:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,128 +460,107 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>